<commit_message>
[IMP] template xlsx export bom
</commit_message>
<xml_diff>
--- a/excel_import_export_bom/import_export_mrp_bom/mrp_bom.xlsx
+++ b/excel_import_export_bom/import_export_mrp_bom/mrp_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Product</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bom Lines / Unit of Measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(bom_line/product_name)</t>
   </si>
 </sst>
 </file>
@@ -221,18 +224,19 @@
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.73"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -256,6 +260,9 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="ALW1" s="0"/>
       <c r="ALX1" s="0"/>

</xml_diff>